<commit_message>
Compoun interest and fee charts
</commit_message>
<xml_diff>
--- a/assets/Charts.xlsx
+++ b/assets/Charts.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Assumption</t>
   </si>
@@ -41,16 +41,7 @@
     <t>ROI</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>ROI 5%</t>
-  </si>
-  <si>
-    <t>ROI 3%</t>
-  </si>
-  <si>
-    <t>ROI 7%</t>
+    <t>Years</t>
   </si>
 </sst>
 </file>
@@ -107,8 +98,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -127,19 +120,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -167,6 +162,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>The development of €10,000 over 40 years</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -212,7 +232,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ROI 3%</c:v>
+                  <c:v>ROI 4%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -248,124 +268,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>10300.0</c:v>
+                  <c:v>10400.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10609.0</c:v>
+                  <c:v>10816.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10927.27</c:v>
+                  <c:v>11248.64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11255.0881</c:v>
+                  <c:v>11698.5856</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11592.740743</c:v>
+                  <c:v>12166.529024</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11940.52296529</c:v>
+                  <c:v>12653.19018496</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12298.7386542487</c:v>
+                  <c:v>13159.3177923584</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12667.70081387616</c:v>
+                  <c:v>13685.69050405274</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13047.73183829244</c:v>
+                  <c:v>14233.11812421485</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13439.16379344122</c:v>
+                  <c:v>14802.44284918345</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13842.33870724445</c:v>
+                  <c:v>15394.54056315078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14257.60886846179</c:v>
+                  <c:v>16010.32218567682</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14685.33713451564</c:v>
+                  <c:v>16650.73507310389</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15125.89724855111</c:v>
+                  <c:v>17316.76447602805</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15579.67416600764</c:v>
+                  <c:v>18009.43505506917</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16047.06439098787</c:v>
+                  <c:v>18729.81245727194</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16528.47632271751</c:v>
+                  <c:v>19479.00495556281</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17024.33061239903</c:v>
+                  <c:v>20258.16515378533</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17535.060530771</c:v>
+                  <c:v>21068.49175993674</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>18061.11234669413</c:v>
+                  <c:v>21911.23143033421</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18602.94571709495</c:v>
+                  <c:v>22787.68068754759</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>19161.0340886078</c:v>
+                  <c:v>23699.18791504949</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>19735.86511126604</c:v>
+                  <c:v>24647.15543165147</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>20327.94106460402</c:v>
+                  <c:v>25633.04164891753</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>20937.77929654214</c:v>
+                  <c:v>26658.36331487423</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>21565.91267543841</c:v>
+                  <c:v>27724.6978474692</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>22212.89005570155</c:v>
+                  <c:v>28833.68576136797</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>22879.2767573726</c:v>
+                  <c:v>29987.0331918227</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>23565.65506009378</c:v>
+                  <c:v>31186.5145194956</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>24272.62471189659</c:v>
+                  <c:v>32433.97510027542</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>25000.8034532535</c:v>
+                  <c:v>33731.33410428644</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>25750.82755685109</c:v>
+                  <c:v>35080.5874684579</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>26523.35238355663</c:v>
+                  <c:v>36483.81096719621</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>27319.05295506332</c:v>
+                  <c:v>37943.16340588407</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>28138.62454371522</c:v>
+                  <c:v>39460.88994211944</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>28982.78328002668</c:v>
+                  <c:v>41039.32553980421</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>29852.26677842748</c:v>
+                  <c:v>42680.89856139638</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>30747.8347817803</c:v>
+                  <c:v>44388.13450385224</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>31670.26982523371</c:v>
+                  <c:v>46163.65988400632</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>32620.37791999072</c:v>
+                  <c:v>48010.2062793666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -396,7 +416,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="square"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
@@ -550,7 +570,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ROI 7%</c:v>
+                  <c:v>ROI 8%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -565,7 +585,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="triangle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
@@ -586,124 +606,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>10700.0</c:v>
+                  <c:v>10800.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11449.0</c:v>
+                  <c:v>11664.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12250.43</c:v>
+                  <c:v>12597.12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13107.9601</c:v>
+                  <c:v>13604.8896</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14025.517307</c:v>
+                  <c:v>14693.280768</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15007.30351849</c:v>
+                  <c:v>15868.74322944001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16057.8147647843</c:v>
+                  <c:v>17138.24268779521</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17181.8617983192</c:v>
+                  <c:v>18509.30210281882</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18384.59212420155</c:v>
+                  <c:v>19990.04627104433</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19671.51357289566</c:v>
+                  <c:v>21589.24997272788</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21048.51952299835</c:v>
+                  <c:v>23316.38997054611</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22521.91588960823</c:v>
+                  <c:v>25181.7011681898</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24098.45000188081</c:v>
+                  <c:v>27196.23726164498</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25785.34150201247</c:v>
+                  <c:v>29371.93624257659</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27590.31540715335</c:v>
+                  <c:v>31721.69114198272</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29521.63748565407</c:v>
+                  <c:v>34259.42643334133</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>31588.15210964986</c:v>
+                  <c:v>37000.18054800864</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>33799.32275732535</c:v>
+                  <c:v>39960.19499184933</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>36165.27535033813</c:v>
+                  <c:v>43157.01059119728</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>38696.8446248618</c:v>
+                  <c:v>46609.57143849306</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41405.62374860212</c:v>
+                  <c:v>50338.33715357251</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44304.01741100427</c:v>
+                  <c:v>54365.40412585832</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>47405.29862977457</c:v>
+                  <c:v>58714.63645592698</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>50723.6695338588</c:v>
+                  <c:v>63411.80737240115</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>54274.32640122891</c:v>
+                  <c:v>68484.75196219324</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>58073.52924931493</c:v>
+                  <c:v>73963.5321191687</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>62138.67629676698</c:v>
+                  <c:v>79880.6146887022</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>66488.38363754067</c:v>
+                  <c:v>86271.06386379837</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>71142.5704921685</c:v>
+                  <c:v>93172.74897290225</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>76122.5504266203</c:v>
+                  <c:v>100626.5688907344</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>81451.12895648374</c:v>
+                  <c:v>108676.6944019932</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>87152.70798343759</c:v>
+                  <c:v>117370.8299541527</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>93253.39754227822</c:v>
+                  <c:v>126760.4963504849</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>99781.1353702377</c:v>
+                  <c:v>136901.3360585237</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>106765.8148461543</c:v>
+                  <c:v>147853.4429432056</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>114239.4218853851</c:v>
+                  <c:v>159681.718378662</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>122236.1814173621</c:v>
+                  <c:v>172456.255848955</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>130792.7141165775</c:v>
+                  <c:v>186252.7563168714</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>139948.204104738</c:v>
+                  <c:v>201152.9768222212</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>149744.5783920695</c:v>
+                  <c:v>217245.2149679989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -730,6 +750,62 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Years</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -794,6 +870,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Portfolio value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -825,6 +957,1157 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="508175376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Development of 10,000 at </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="mr-IN"/>
+              <a:t>ROI 4%</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ROI 4%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>10400.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10816.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11248.64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11698.5856</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12166.529024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12653.19018496</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13159.3177923584</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13685.69050405274</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14233.11812421485</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14802.44284918345</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15394.54056315078</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16010.32218567682</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16650.73507310389</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17316.76447602805</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18009.43505506917</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18729.81245727194</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19479.00495556281</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20258.16515378533</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>21068.49175993674</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21911.23143033421</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22787.68068754759</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23699.18791504949</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24647.15543165147</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25633.04164891753</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26658.36331487423</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>27724.6978474692</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>28833.68576136797</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29987.0331918227</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>31186.5145194956</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>32433.97510027542</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>33731.33410428644</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>35080.5874684579</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>36483.81096719621</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>37943.16340588407</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>39460.88994211944</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>41039.32553980421</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>42680.89856139638</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44388.13450385224</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>46163.65988400632</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>48010.2062793666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="508469984"/>
+        <c:axId val="508187536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="508469984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="508187536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="508187536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Portfolio value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="508469984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Development of €10,000 over 10 years</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ROI 4%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10400.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10816.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11248.64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11698.5856</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12166.529024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12653.19018496</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13159.3177923584</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13685.69050405274</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14233.11812421485</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14802.44284918345</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ROI 5%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="flat">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:bevel/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="sq">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:bevel/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11025.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11576.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12155.0625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12762.815625</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13400.95640625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14071.0042265625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14774.55443789063</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15513.28215978516</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16288.94626777442</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ROI 8%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10800.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11664.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12597.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13604.8896</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14693.280768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15868.74322944001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17138.24268779521</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18509.30210281882</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19990.04627104433</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21589.24997272788</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="262291664"/>
+        <c:axId val="755689824"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="262291664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Years</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="755689824"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="755689824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Portfolio value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="262291664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -945,7 +2228,1093 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1475,6 +3844,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1748,8 +4177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="113" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1764,14 +4193,17 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
+      <c r="F1" s="2" t="str">
+        <f>CONCATENATE("ROI ",TEXT(B3,"0%"))</f>
+        <v>ROI 4%</v>
+      </c>
+      <c r="G1" s="2" t="str">
+        <f>CONCATENATE("ROI ",TEXT(B4,"0%"))</f>
+        <v>ROI 5%</v>
+      </c>
+      <c r="H1" s="2" t="str">
+        <f>CONCATENATE("ROI ",TEXT(B5,"0%"))</f>
+        <v>ROI 8%</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1786,7 +4218,7 @@
       </c>
       <c r="F2">
         <f>SUM(B$2*(1+B$3)^E2)</f>
-        <v>10300</v>
+        <v>10400</v>
       </c>
       <c r="G2">
         <f>SUM(B$2*(1+B$4)^E2)</f>
@@ -1794,7 +4226,7 @@
       </c>
       <c r="H2">
         <f>SUM(B$2*(1+B$5)^E2)</f>
-        <v>10700</v>
+        <v>10800</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1802,7 +4234,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="E3">
         <f>SUM(E2+1)</f>
@@ -1810,7 +4242,7 @@
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F41" si="0">SUM(B$2*(1+B$3)^E3)</f>
-        <v>10609</v>
+        <v>10816.000000000002</v>
       </c>
       <c r="G3">
         <f>SUM(B$2*(1+B$4)^E3)</f>
@@ -1818,7 +4250,7 @@
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H41" si="1">SUM(B$2*(1+B$5)^E3)</f>
-        <v>11449</v>
+        <v>11664.000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1834,7 +4266,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>10927.27</v>
+        <v>11248.640000000001</v>
       </c>
       <c r="G4">
         <f>SUM(B$2*(1+B$4)^E4)</f>
@@ -1842,7 +4274,7 @@
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
-        <v>12250.43</v>
+        <v>12597.12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1850,7 +4282,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
@@ -1858,7 +4290,7 @@
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>11255.088099999999</v>
+        <v>11698.585600000002</v>
       </c>
       <c r="G5">
         <f>SUM(B$2*(1+B$4)^E5)</f>
@@ -1866,7 +4298,7 @@
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>13107.9601</v>
+        <v>13604.889600000002</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1876,7 +4308,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>11592.740742999998</v>
+        <v>12166.529024000003</v>
       </c>
       <c r="G6">
         <f>SUM(B$2*(1+B$4)^E6)</f>
@@ -1884,7 +4316,7 @@
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>14025.517307000002</v>
+        <v>14693.280768000004</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1894,7 +4326,7 @@
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>11940.52296529</v>
+        <v>12653.190184960004</v>
       </c>
       <c r="G7">
         <f>SUM(B$2*(1+B$4)^E7)</f>
@@ -1902,7 +4334,7 @@
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>15007.30351849</v>
+        <v>15868.743229440006</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1912,7 +4344,7 @@
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>12298.7386542487</v>
+        <v>13159.317792358403</v>
       </c>
       <c r="G8">
         <f>SUM(B$2*(1+B$4)^E8)</f>
@@ -1920,7 +4352,7 @@
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>16057.814764784302</v>
+        <v>17138.242687795206</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1930,7 +4362,7 @@
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>12667.700813876159</v>
+        <v>13685.690504052742</v>
       </c>
       <c r="G9">
         <f>SUM(B$2*(1+B$4)^E9)</f>
@@ -1938,7 +4370,7 @@
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>17181.861798319202</v>
+        <v>18509.302102818823</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1948,7 +4380,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>13047.731838292444</v>
+        <v>14233.118124214852</v>
       </c>
       <c r="G10">
         <f>SUM(B$2*(1+B$4)^E10)</f>
@@ -1956,7 +4388,7 @@
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>18384.59212420155</v>
+        <v>19990.046271044332</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1966,7 +4398,7 @@
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>13439.163793441217</v>
+        <v>14802.442849183446</v>
       </c>
       <c r="G11">
         <f>SUM(B$2*(1+B$4)^E11)</f>
@@ -1974,7 +4406,7 @@
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>19671.513572895656</v>
+        <v>21589.249972727877</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1984,7 +4416,7 @@
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>13842.338707244455</v>
+        <v>15394.540563150782</v>
       </c>
       <c r="G12">
         <f>SUM(B$2*(1+B$4)^E12)</f>
@@ -1992,7 +4424,7 @@
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>21048.519522998355</v>
+        <v>23316.389970546108</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -2002,7 +4434,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>14257.608868461786</v>
+        <v>16010.322185676818</v>
       </c>
       <c r="G13">
         <f>SUM(B$2*(1+B$4)^E13)</f>
@@ -2010,7 +4442,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>22521.915889608234</v>
+        <v>25181.7011681898</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -2020,7 +4452,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>14685.337134515639</v>
+        <v>16650.73507310389</v>
       </c>
       <c r="G14">
         <f>SUM(B$2*(1+B$4)^E14)</f>
@@ -2028,7 +4460,7 @@
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
-        <v>24098.450001880814</v>
+        <v>27196.237261644983</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -2038,7 +4470,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>15125.897248551109</v>
+        <v>17316.764476028045</v>
       </c>
       <c r="G15">
         <f>SUM(B$2*(1+B$4)^E15)</f>
@@ -2046,7 +4478,7 @@
       </c>
       <c r="H15">
         <f t="shared" si="1"/>
-        <v>25785.34150201247</v>
+        <v>29371.936242576587</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -2056,7 +4488,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>15579.674166007644</v>
+        <v>18009.435055069167</v>
       </c>
       <c r="G16">
         <f>SUM(B$2*(1+B$4)^E16)</f>
@@ -2064,7 +4496,7 @@
       </c>
       <c r="H16">
         <f t="shared" si="1"/>
-        <v>27590.315407153346</v>
+        <v>31721.691141982716</v>
       </c>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.2">
@@ -2074,7 +4506,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>16047.064390987871</v>
+        <v>18729.812457271939</v>
       </c>
       <c r="G17">
         <f>SUM(B$2*(1+B$4)^E17)</f>
@@ -2082,7 +4514,7 @@
       </c>
       <c r="H17">
         <f t="shared" si="1"/>
-        <v>29521.637485654075</v>
+        <v>34259.42643334133</v>
       </c>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.2">
@@ -2092,7 +4524,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>16528.476322717506</v>
+        <v>19479.004955562814</v>
       </c>
       <c r="G18">
         <f>SUM(B$2*(1+B$4)^E18)</f>
@@ -2100,7 +4532,7 @@
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
-        <v>31588.152109649862</v>
+        <v>37000.18054800864</v>
       </c>
     </row>
     <row r="19" spans="5:8" x14ac:dyDescent="0.2">
@@ -2110,7 +4542,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>17024.330612399033</v>
+        <v>20258.165153785329</v>
       </c>
       <c r="G19">
         <f>SUM(B$2*(1+B$4)^E19)</f>
@@ -2118,7 +4550,7 @@
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
-        <v>33799.322757325353</v>
+        <v>39960.194991849334</v>
       </c>
     </row>
     <row r="20" spans="5:8" x14ac:dyDescent="0.2">
@@ -2128,7 +4560,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>17535.060530771003</v>
+        <v>21068.491759936744</v>
       </c>
       <c r="G20">
         <f>SUM(B$2*(1+B$4)^E20)</f>
@@ -2136,7 +4568,7 @@
       </c>
       <c r="H20">
         <f t="shared" si="1"/>
-        <v>36165.275350338132</v>
+        <v>43157.010591197286</v>
       </c>
     </row>
     <row r="21" spans="5:8" x14ac:dyDescent="0.2">
@@ -2146,7 +4578,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>18061.112346694132</v>
+        <v>21911.231430334214</v>
       </c>
       <c r="G21">
         <f>SUM(B$2*(1+B$4)^E21)</f>
@@ -2154,7 +4586,7 @@
       </c>
       <c r="H21">
         <f t="shared" si="1"/>
-        <v>38696.844624861798</v>
+        <v>46609.571438493062</v>
       </c>
     </row>
     <row r="22" spans="5:8" x14ac:dyDescent="0.2">
@@ -2164,7 +4596,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>18602.945717094954</v>
+        <v>22787.680687547589</v>
       </c>
       <c r="G22">
         <f>SUM(B$2*(1+B$4)^E22)</f>
@@ -2172,7 +4604,7 @@
       </c>
       <c r="H22">
         <f t="shared" si="1"/>
-        <v>41405.62374860212</v>
+        <v>50338.337153572509</v>
       </c>
     </row>
     <row r="23" spans="5:8" x14ac:dyDescent="0.2">
@@ -2182,7 +4614,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>19161.034088607805</v>
+        <v>23699.18791504949</v>
       </c>
       <c r="G23">
         <f>SUM(B$2*(1+B$4)^E23)</f>
@@ -2190,7 +4622,7 @@
       </c>
       <c r="H23">
         <f t="shared" si="1"/>
-        <v>44304.017411004272</v>
+        <v>54365.404125858324</v>
       </c>
     </row>
     <row r="24" spans="5:8" x14ac:dyDescent="0.2">
@@ -2200,7 +4632,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>19735.865111266041</v>
+        <v>24647.155431651467</v>
       </c>
       <c r="G24">
         <f>SUM(B$2*(1+B$4)^E24)</f>
@@ -2208,7 +4640,7 @@
       </c>
       <c r="H24">
         <f t="shared" si="1"/>
-        <v>47405.298629774574</v>
+        <v>58714.636455926986</v>
       </c>
     </row>
     <row r="25" spans="5:8" x14ac:dyDescent="0.2">
@@ -2218,7 +4650,7 @@
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>20327.94106460402</v>
+        <v>25633.041648917526</v>
       </c>
       <c r="G25">
         <f>SUM(B$2*(1+B$4)^E25)</f>
@@ -2226,7 +4658,7 @@
       </c>
       <c r="H25">
         <f t="shared" si="1"/>
-        <v>50723.669533858796</v>
+        <v>63411.807372401148</v>
       </c>
     </row>
     <row r="26" spans="5:8" x14ac:dyDescent="0.2">
@@ -2236,7 +4668,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>20937.779296542139</v>
+        <v>26658.363314874234</v>
       </c>
       <c r="G26">
         <f>SUM(B$2*(1+B$4)^E26)</f>
@@ -2244,7 +4676,7 @@
       </c>
       <c r="H26">
         <f t="shared" si="1"/>
-        <v>54274.326401228915</v>
+        <v>68484.751962193244</v>
       </c>
     </row>
     <row r="27" spans="5:8" x14ac:dyDescent="0.2">
@@ -2254,7 +4686,7 @@
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>21565.912675438405</v>
+        <v>27724.6978474692</v>
       </c>
       <c r="G27">
         <f>SUM(B$2*(1+B$4)^E27)</f>
@@ -2262,7 +4694,7 @@
       </c>
       <c r="H27">
         <f t="shared" si="1"/>
-        <v>58073.529249314932</v>
+        <v>73963.532119168696</v>
       </c>
     </row>
     <row r="28" spans="5:8" x14ac:dyDescent="0.2">
@@ -2272,7 +4704,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>22212.890055701555</v>
+        <v>28833.685761367968</v>
       </c>
       <c r="G28">
         <f>SUM(B$2*(1+B$4)^E28)</f>
@@ -2280,7 +4712,7 @@
       </c>
       <c r="H28">
         <f t="shared" si="1"/>
-        <v>62138.676296766986</v>
+        <v>79880.614688702204</v>
       </c>
     </row>
     <row r="29" spans="5:8" x14ac:dyDescent="0.2">
@@ -2290,7 +4722,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>22879.276757372601</v>
+        <v>29987.033191822695</v>
       </c>
       <c r="G29">
         <f>SUM(B$2*(1+B$4)^E29)</f>
@@ -2298,7 +4730,7 @@
       </c>
       <c r="H29">
         <f t="shared" si="1"/>
-        <v>66488.383637540668</v>
+        <v>86271.063863798379</v>
       </c>
     </row>
     <row r="30" spans="5:8" x14ac:dyDescent="0.2">
@@ -2308,7 +4740,7 @@
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>23565.655060093777</v>
+        <v>31186.514519495602</v>
       </c>
       <c r="G30">
         <f>SUM(B$2*(1+B$4)^E30)</f>
@@ -2316,7 +4748,7 @@
       </c>
       <c r="H30">
         <f t="shared" si="1"/>
-        <v>71142.57049216851</v>
+        <v>93172.748972902249</v>
       </c>
     </row>
     <row r="31" spans="5:8" x14ac:dyDescent="0.2">
@@ -2326,7 +4758,7 @@
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>24272.624711896591</v>
+        <v>32433.975100275424</v>
       </c>
       <c r="G31">
         <f>SUM(B$2*(1+B$4)^E31)</f>
@@ -2334,7 +4766,7 @@
       </c>
       <c r="H31">
         <f t="shared" si="1"/>
-        <v>76122.550426620306</v>
+        <v>100626.56889073444</v>
       </c>
     </row>
     <row r="32" spans="5:8" x14ac:dyDescent="0.2">
@@ -2344,7 +4776,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>25000.803453253491</v>
+        <v>33731.334104286441</v>
       </c>
       <c r="G32">
         <f>SUM(B$2*(1+B$4)^E32)</f>
@@ -2352,7 +4784,7 @@
       </c>
       <c r="H32">
         <f t="shared" si="1"/>
-        <v>81451.12895648375</v>
+        <v>108676.69440199321</v>
       </c>
     </row>
     <row r="33" spans="5:8" x14ac:dyDescent="0.2">
@@ -2362,7 +4794,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>25750.827556851091</v>
+        <v>35080.587468457903</v>
       </c>
       <c r="G33">
         <f>SUM(B$2*(1+B$4)^E33)</f>
@@ -2370,7 +4802,7 @@
       </c>
       <c r="H33">
         <f t="shared" si="1"/>
-        <v>87152.707983437591</v>
+        <v>117370.82995415268</v>
       </c>
     </row>
     <row r="34" spans="5:8" x14ac:dyDescent="0.2">
@@ -2380,7 +4812,7 @@
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
-        <v>26523.352383556627</v>
+        <v>36483.810967196216</v>
       </c>
       <c r="G34">
         <f>SUM(B$2*(1+B$4)^E34)</f>
@@ -2388,7 +4820,7 @@
       </c>
       <c r="H34">
         <f t="shared" si="1"/>
-        <v>93253.397542278224</v>
+        <v>126760.49635048489</v>
       </c>
     </row>
     <row r="35" spans="5:8" x14ac:dyDescent="0.2">
@@ -2398,7 +4830,7 @@
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>27319.052955063322</v>
+        <v>37943.163405884072</v>
       </c>
       <c r="G35">
         <f>SUM(B$2*(1+B$4)^E35)</f>
@@ -2406,7 +4838,7 @@
       </c>
       <c r="H35">
         <f t="shared" si="1"/>
-        <v>99781.135370237695</v>
+        <v>136901.33605852368</v>
       </c>
     </row>
     <row r="36" spans="5:8" x14ac:dyDescent="0.2">
@@ -2416,7 +4848,7 @@
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>28138.624543715225</v>
+        <v>39460.889942119436</v>
       </c>
       <c r="G36">
         <f>SUM(B$2*(1+B$4)^E36)</f>
@@ -2424,7 +4856,7 @@
       </c>
       <c r="H36">
         <f t="shared" si="1"/>
-        <v>106765.81484615435</v>
+        <v>147853.44294320559</v>
       </c>
     </row>
     <row r="37" spans="5:8" x14ac:dyDescent="0.2">
@@ -2434,7 +4866,7 @@
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>28982.783280026681</v>
+        <v>41039.325539804209</v>
       </c>
       <c r="G37">
         <f>SUM(B$2*(1+B$4)^E37)</f>
@@ -2442,7 +4874,7 @@
       </c>
       <c r="H37">
         <f t="shared" si="1"/>
-        <v>114239.42188538515</v>
+        <v>159681.71837866207</v>
       </c>
     </row>
     <row r="38" spans="5:8" x14ac:dyDescent="0.2">
@@ -2452,7 +4884,7 @@
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
-        <v>29852.266778427478</v>
+        <v>42680.898561396389</v>
       </c>
       <c r="G38">
         <f>SUM(B$2*(1+B$4)^E38)</f>
@@ -2460,7 +4892,7 @@
       </c>
       <c r="H38">
         <f t="shared" si="1"/>
-        <v>122236.18141736212</v>
+        <v>172456.25584895504</v>
       </c>
     </row>
     <row r="39" spans="5:8" x14ac:dyDescent="0.2">
@@ -2470,7 +4902,7 @@
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
-        <v>30747.834781780301</v>
+        <v>44388.134503852241</v>
       </c>
       <c r="G39">
         <f>SUM(B$2*(1+B$4)^E39)</f>
@@ -2478,7 +4910,7 @@
       </c>
       <c r="H39">
         <f t="shared" si="1"/>
-        <v>130792.71411657747</v>
+        <v>186252.75631687144</v>
       </c>
     </row>
     <row r="40" spans="5:8" x14ac:dyDescent="0.2">
@@ -2488,7 +4920,7 @@
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
-        <v>31670.269825233714</v>
+        <v>46163.659884006323</v>
       </c>
       <c r="G40">
         <f>SUM(B$2*(1+B$4)^E40)</f>
@@ -2496,7 +4928,7 @@
       </c>
       <c r="H40">
         <f t="shared" si="1"/>
-        <v>139948.2041047379</v>
+        <v>201152.97682222116</v>
       </c>
     </row>
     <row r="41" spans="5:8" x14ac:dyDescent="0.2">
@@ -2506,7 +4938,7 @@
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
-        <v>32620.377919990719</v>
+        <v>48010.206279366597</v>
       </c>
       <c r="G41">
         <f>SUM(B$2*(1+B$4)^E41)</f>
@@ -2514,7 +4946,7 @@
       </c>
       <c r="H41">
         <f t="shared" si="1"/>
-        <v>149744.57839206952</v>
+        <v>217245.21496799888</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Exercise and ACH chart
</commit_message>
<xml_diff>
--- a/assets/Charts.xlsx
+++ b/assets/Charts.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mentor/Dev/immortal-millionaire/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mentor/dev/immortal-millionaire/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FInance" sheetId="1" r:id="rId1"/>
+    <sheet name="Health" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Assumption</t>
   </si>
@@ -42,6 +43,54 @@
   </si>
   <si>
     <t>Years</t>
+  </si>
+  <si>
+    <t>MVPA</t>
+  </si>
+  <si>
+    <t>VPA</t>
+  </si>
+  <si>
+    <t>Improvement</t>
+  </si>
+  <si>
+    <t>10-150</t>
+  </si>
+  <si>
+    <t>40.4%</t>
+  </si>
+  <si>
+    <t>150-299</t>
+  </si>
+  <si>
+    <t>47.5%</t>
+  </si>
+  <si>
+    <t>77.3%</t>
+  </si>
+  <si>
+    <t>10-150 moderate</t>
+  </si>
+  <si>
+    <t>150-299 moderate</t>
+  </si>
+  <si>
+    <t>300+ moderate</t>
+  </si>
+  <si>
+    <t>10-150 moderate
+of which 30+ vigorous</t>
+  </si>
+  <si>
+    <t>150-299 moderate
+of which 30+ vigorous</t>
+  </si>
+  <si>
+    <t>300+ moderate
+of which 30+ vigorous</t>
+  </si>
+  <si>
+    <t>0 exercise (baseline)</t>
   </si>
 </sst>
 </file>
@@ -98,7 +147,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -114,13 +163,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -128,6 +187,9 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -135,6 +197,9 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -228,7 +293,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>FInance!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -263,7 +328,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$41</c:f>
+              <c:f>FInance!$F$2:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
@@ -397,7 +462,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>FInance!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -432,7 +497,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$41</c:f>
+              <c:f>FInance!$G$2:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
@@ -566,7 +631,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>FInance!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -601,7 +666,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$41</c:f>
+              <c:f>FInance!$H$2:$H$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
@@ -740,11 +805,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="508175376"/>
-        <c:axId val="725410608"/>
+        <c:axId val="-19949088"/>
+        <c:axId val="-19944976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="508175376"/>
+        <c:axId val="-19949088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,7 +907,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="725410608"/>
+        <c:crossAx val="-19944976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -850,7 +915,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="725410608"/>
+        <c:axId val="-19944976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,7 +1021,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="508175376"/>
+        <c:crossAx val="-19949088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1081,7 +1146,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1122,7 +1186,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>FInance!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1157,7 +1221,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$41</c:f>
+              <c:f>FInance!$F$2:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
@@ -1296,11 +1360,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="508469984"/>
-        <c:axId val="508187536"/>
+        <c:axId val="79699072"/>
+        <c:axId val="79702192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="508469984"/>
+        <c:axId val="79699072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1332,7 +1396,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1398,7 +1461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="508187536"/>
+        <c:crossAx val="79702192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1406,7 +1469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="508187536"/>
+        <c:axId val="79702192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1452,7 +1515,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1512,7 +1574,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="508469984"/>
+        <c:crossAx val="79699072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1648,7 +1710,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>FInance!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1683,7 +1745,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$11</c:f>
+              <c:f>FInance!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1727,7 +1789,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>FInance!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1763,7 +1825,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$11</c:f>
+              <c:f>FInance!$G$2:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1807,7 +1869,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>FInance!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1842,7 +1904,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$11</c:f>
+              <c:f>FInance!$H$2:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1891,11 +1953,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="262291664"/>
-        <c:axId val="755689824"/>
+        <c:axId val="79733328"/>
+        <c:axId val="79737088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="262291664"/>
+        <c:axId val="79733328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1993,7 +2055,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="755689824"/>
+        <c:crossAx val="79737088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2001,7 +2063,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="755689824"/>
+        <c:axId val="79737088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2107,7 +2169,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262291664"/>
+        <c:crossAx val="79733328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2151,6 +2213,498 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>The % improvement</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>exercise has on all-cause</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> mortality</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Health!$D$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Improvement</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Health!$C$13:$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0 exercise (baseline)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10-150 moderate</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10-150 moderate_x000d_of which 30+ vigorous</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150-299 moderate</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150-299 moderate_x000d_of which 30+ vigorous</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300+ moderate</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300+ moderate_x000d_of which 30+ vigorous</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Health!$D$13:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>77.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="130355568"/>
+        <c:axId val="130357344"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="130355568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Minutes of exercise per week</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="130357344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="130357344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Improvement in All-Cause mortality in %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="130355568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2308,6 +2862,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -3316,6 +3910,509 @@
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3904,6 +5001,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>683699</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>158988</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>772599</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>60062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4177,7 +5309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="113" workbookViewId="0">
+    <sheetView topLeftCell="C2" zoomScale="113" workbookViewId="0">
       <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
@@ -4221,7 +5353,7 @@
         <v>10400</v>
       </c>
       <c r="G2">
-        <f>SUM(B$2*(1+B$4)^E2)</f>
+        <f t="shared" ref="G2:G41" si="0">SUM(B$2*(1+B$4)^E2)</f>
         <v>10500</v>
       </c>
       <c r="H2">
@@ -4241,15 +5373,15 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F41" si="0">SUM(B$2*(1+B$3)^E3)</f>
+        <f t="shared" ref="F3:F41" si="1">SUM(B$2*(1+B$3)^E3)</f>
         <v>10816.000000000002</v>
       </c>
       <c r="G3">
-        <f>SUM(B$2*(1+B$4)^E3)</f>
+        <f t="shared" si="0"/>
         <v>11025</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H41" si="1">SUM(B$2*(1+B$5)^E3)</f>
+        <f t="shared" ref="H3:H41" si="2">SUM(B$2*(1+B$5)^E3)</f>
         <v>11664.000000000002</v>
       </c>
     </row>
@@ -4261,19 +5393,19 @@
         <v>0.05</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E41" si="2">SUM(E3+1)</f>
+        <f t="shared" ref="E4:E41" si="3">SUM(E3+1)</f>
         <v>3</v>
       </c>
       <c r="F4">
+        <f t="shared" si="1"/>
+        <v>11248.640000000001</v>
+      </c>
+      <c r="G4">
         <f t="shared" si="0"/>
-        <v>11248.640000000001</v>
-      </c>
-      <c r="G4">
-        <f>SUM(B$2*(1+B$4)^E4)</f>
         <v>11576.250000000002</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12597.12</v>
       </c>
     </row>
@@ -4285,668 +5417,888 @@
         <v>0.08</v>
       </c>
       <c r="E5">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>11698.585600000002</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>12155.0625</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>11698.585600000002</v>
-      </c>
-      <c r="G5">
-        <f>SUM(B$2*(1+B$4)^E5)</f>
-        <v>12155.0625</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
         <v>13604.889600000002</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E6">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>12166.529024000003</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>12762.815625000001</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>12166.529024000003</v>
-      </c>
-      <c r="G6">
-        <f>SUM(B$2*(1+B$4)^E6)</f>
-        <v>12762.815625000001</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
         <v>14693.280768000004</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>12653.190184960004</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>13400.956406249999</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>12653.190184960004</v>
-      </c>
-      <c r="G7">
-        <f>SUM(B$2*(1+B$4)^E7)</f>
-        <v>13400.956406249999</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
         <v>15868.743229440006</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E8">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>13159.317792358403</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>14071.004226562502</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>13159.317792358403</v>
-      </c>
-      <c r="G8">
-        <f>SUM(B$2*(1+B$4)^E8)</f>
-        <v>14071.004226562502</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
         <v>17138.242687795206</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E9">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>13685.690504052742</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>14774.554437890625</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>13685.690504052742</v>
-      </c>
-      <c r="G9">
-        <f>SUM(B$2*(1+B$4)^E9)</f>
-        <v>14774.554437890625</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
         <v>18509.302102818823</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E10">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>14233.118124214852</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>15513.282159785158</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>14233.118124214852</v>
-      </c>
-      <c r="G10">
-        <f>SUM(B$2*(1+B$4)^E10)</f>
-        <v>15513.282159785158</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
         <v>19990.046271044332</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E11">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>14802.442849183446</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>16288.946267774416</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>14802.442849183446</v>
-      </c>
-      <c r="G11">
-        <f>SUM(B$2*(1+B$4)^E11)</f>
-        <v>16288.946267774416</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="1"/>
         <v>21589.249972727877</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E12">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>15394.540563150782</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>17103.393581163138</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>15394.540563150782</v>
-      </c>
-      <c r="G12">
-        <f>SUM(B$2*(1+B$4)^E12)</f>
-        <v>17103.393581163138</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="1"/>
         <v>23316.389970546108</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E13">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>16010.322185676818</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>17958.563260221294</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>16010.322185676818</v>
-      </c>
-      <c r="G13">
-        <f>SUM(B$2*(1+B$4)^E13)</f>
-        <v>17958.563260221294</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
         <v>25181.7011681898</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E14">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>16650.73507310389</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>18856.491423232361</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>16650.73507310389</v>
-      </c>
-      <c r="G14">
-        <f>SUM(B$2*(1+B$4)^E14)</f>
-        <v>18856.491423232361</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
         <v>27196.237261644983</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E15">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>17316.764476028045</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>19799.315994393972</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>17316.764476028045</v>
-      </c>
-      <c r="G15">
-        <f>SUM(B$2*(1+B$4)^E15)</f>
-        <v>19799.315994393972</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="1"/>
         <v>29371.936242576587</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E16">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>18009.435055069167</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>20789.281794113678</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>18009.435055069167</v>
-      </c>
-      <c r="G16">
-        <f>SUM(B$2*(1+B$4)^E16)</f>
-        <v>20789.281794113678</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="1"/>
         <v>31721.691141982716</v>
       </c>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E17">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>18729.812457271939</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>21828.74588381936</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>18729.812457271939</v>
-      </c>
-      <c r="G17">
-        <f>SUM(B$2*(1+B$4)^E17)</f>
-        <v>21828.74588381936</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="1"/>
         <v>34259.42643334133</v>
       </c>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E18">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>19479.004955562814</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>22920.183178010331</v>
+      </c>
+      <c r="H18">
         <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>19479.004955562814</v>
-      </c>
-      <c r="G18">
-        <f>SUM(B$2*(1+B$4)^E18)</f>
-        <v>22920.183178010331</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="1"/>
         <v>37000.18054800864</v>
       </c>
     </row>
     <row r="19" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E19">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>20258.165153785329</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>24066.192336910848</v>
+      </c>
+      <c r="H19">
         <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>20258.165153785329</v>
-      </c>
-      <c r="G19">
-        <f>SUM(B$2*(1+B$4)^E19)</f>
-        <v>24066.192336910848</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="1"/>
         <v>39960.194991849334</v>
       </c>
     </row>
     <row r="20" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E20">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>21068.491759936744</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>25269.501953756389</v>
+      </c>
+      <c r="H20">
         <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>21068.491759936744</v>
-      </c>
-      <c r="G20">
-        <f>SUM(B$2*(1+B$4)^E20)</f>
-        <v>25269.501953756389</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="1"/>
         <v>43157.010591197286</v>
       </c>
     </row>
     <row r="21" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E21">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>21911.231430334214</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>26532.97705144421</v>
+      </c>
+      <c r="H21">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>21911.231430334214</v>
-      </c>
-      <c r="G21">
-        <f>SUM(B$2*(1+B$4)^E21)</f>
-        <v>26532.97705144421</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="1"/>
         <v>46609.571438493062</v>
       </c>
     </row>
     <row r="22" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E22">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>22787.680687547589</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>27859.625904016419</v>
+      </c>
+      <c r="H22">
         <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>22787.680687547589</v>
-      </c>
-      <c r="G22">
-        <f>SUM(B$2*(1+B$4)^E22)</f>
-        <v>27859.625904016419</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="1"/>
         <v>50338.337153572509</v>
       </c>
     </row>
     <row r="23" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E23">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>23699.18791504949</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>29252.607199217236</v>
+      </c>
+      <c r="H23">
         <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>23699.18791504949</v>
-      </c>
-      <c r="G23">
-        <f>SUM(B$2*(1+B$4)^E23)</f>
-        <v>29252.607199217236</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="1"/>
         <v>54365.404125858324</v>
       </c>
     </row>
     <row r="24" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E24">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>24647.155431651467</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>30715.237559178106</v>
+      </c>
+      <c r="H24">
         <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="0"/>
-        <v>24647.155431651467</v>
-      </c>
-      <c r="G24">
-        <f>SUM(B$2*(1+B$4)^E24)</f>
-        <v>30715.237559178106</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="1"/>
         <v>58714.636455926986</v>
       </c>
     </row>
     <row r="25" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E25">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>25633.041648917526</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>32250.999437137008</v>
+      </c>
+      <c r="H25">
         <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="0"/>
-        <v>25633.041648917526</v>
-      </c>
-      <c r="G25">
-        <f>SUM(B$2*(1+B$4)^E25)</f>
-        <v>32250.999437137008</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="1"/>
         <v>63411.807372401148</v>
       </c>
     </row>
     <row r="26" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E26">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>26658.363314874234</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>33863.549408993858</v>
+      </c>
+      <c r="H26">
         <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="0"/>
-        <v>26658.363314874234</v>
-      </c>
-      <c r="G26">
-        <f>SUM(B$2*(1+B$4)^E26)</f>
-        <v>33863.549408993858</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="1"/>
         <v>68484.751962193244</v>
       </c>
     </row>
     <row r="27" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E27">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>27724.6978474692</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>35556.726879443551</v>
+      </c>
+      <c r="H27">
         <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="0"/>
-        <v>27724.6978474692</v>
-      </c>
-      <c r="G27">
-        <f>SUM(B$2*(1+B$4)^E27)</f>
-        <v>35556.726879443551</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="1"/>
         <v>73963.532119168696</v>
       </c>
     </row>
     <row r="28" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E28">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>28833.685761367968</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>37334.563223415731</v>
+      </c>
+      <c r="H28">
         <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="0"/>
-        <v>28833.685761367968</v>
-      </c>
-      <c r="G28">
-        <f>SUM(B$2*(1+B$4)^E28)</f>
-        <v>37334.563223415731</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="1"/>
         <v>79880.614688702204</v>
       </c>
     </row>
     <row r="29" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E29">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>29987.033191822695</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>39201.291384586511</v>
+      </c>
+      <c r="H29">
         <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="0"/>
-        <v>29987.033191822695</v>
-      </c>
-      <c r="G29">
-        <f>SUM(B$2*(1+B$4)^E29)</f>
-        <v>39201.291384586511</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="1"/>
         <v>86271.063863798379</v>
       </c>
     </row>
     <row r="30" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E30">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>31186.514519495602</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>41161.355953815852</v>
+      </c>
+      <c r="H30">
         <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="0"/>
-        <v>31186.514519495602</v>
-      </c>
-      <c r="G30">
-        <f>SUM(B$2*(1+B$4)^E30)</f>
-        <v>41161.355953815852</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="1"/>
         <v>93172.748972902249</v>
       </c>
     </row>
     <row r="31" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E31">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>32433.975100275424</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>43219.423751506627</v>
+      </c>
+      <c r="H31">
         <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="0"/>
-        <v>32433.975100275424</v>
-      </c>
-      <c r="G31">
-        <f>SUM(B$2*(1+B$4)^E31)</f>
-        <v>43219.423751506627</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="1"/>
         <v>100626.56889073444</v>
       </c>
     </row>
     <row r="32" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E32">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>33731.334104286441</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>45380.394939081976</v>
+      </c>
+      <c r="H32">
         <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="0"/>
-        <v>33731.334104286441</v>
-      </c>
-      <c r="G32">
-        <f>SUM(B$2*(1+B$4)^E32)</f>
-        <v>45380.394939081976</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="1"/>
         <v>108676.69440199321</v>
       </c>
     </row>
     <row r="33" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E33">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>35080.587468457903</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>47649.414686036071</v>
+      </c>
+      <c r="H33">
         <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="0"/>
-        <v>35080.587468457903</v>
-      </c>
-      <c r="G33">
-        <f>SUM(B$2*(1+B$4)^E33)</f>
-        <v>47649.414686036071</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="1"/>
         <v>117370.82995415268</v>
       </c>
     </row>
     <row r="34" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E34">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>36483.810967196216</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>50031.885420337872</v>
+      </c>
+      <c r="H34">
         <f t="shared" si="2"/>
-        <v>33</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="0"/>
-        <v>36483.810967196216</v>
-      </c>
-      <c r="G34">
-        <f>SUM(B$2*(1+B$4)^E34)</f>
-        <v>50031.885420337872</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="1"/>
         <v>126760.49635048489</v>
       </c>
     </row>
     <row r="35" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E35">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>37943.163405884072</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>52533.479691354769</v>
+      </c>
+      <c r="H35">
         <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="0"/>
-        <v>37943.163405884072</v>
-      </c>
-      <c r="G35">
-        <f>SUM(B$2*(1+B$4)^E35)</f>
-        <v>52533.479691354769</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="1"/>
         <v>136901.33605852368</v>
       </c>
     </row>
     <row r="36" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E36">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>39460.889942119436</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>55160.153675922513</v>
+      </c>
+      <c r="H36">
         <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="0"/>
-        <v>39460.889942119436</v>
-      </c>
-      <c r="G36">
-        <f>SUM(B$2*(1+B$4)^E36)</f>
-        <v>55160.153675922513</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="1"/>
         <v>147853.44294320559</v>
       </c>
     </row>
     <row r="37" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E37">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>41039.325539804209</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>57918.16135971863</v>
+      </c>
+      <c r="H37">
         <f t="shared" si="2"/>
-        <v>36</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="0"/>
-        <v>41039.325539804209</v>
-      </c>
-      <c r="G37">
-        <f>SUM(B$2*(1+B$4)^E37)</f>
-        <v>57918.16135971863</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="1"/>
         <v>159681.71837866207</v>
       </c>
     </row>
     <row r="38" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E38">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>42680.898561396389</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>60814.06942770457</v>
+      </c>
+      <c r="H38">
         <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="0"/>
-        <v>42680.898561396389</v>
-      </c>
-      <c r="G38">
-        <f>SUM(B$2*(1+B$4)^E38)</f>
-        <v>60814.06942770457</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="1"/>
         <v>172456.25584895504</v>
       </c>
     </row>
     <row r="39" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E39">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>44388.134503852241</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>63854.772899089781</v>
+      </c>
+      <c r="H39">
         <f t="shared" si="2"/>
-        <v>38</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="0"/>
-        <v>44388.134503852241</v>
-      </c>
-      <c r="G39">
-        <f>SUM(B$2*(1+B$4)^E39)</f>
-        <v>63854.772899089781</v>
-      </c>
-      <c r="H39">
-        <f t="shared" si="1"/>
         <v>186252.75631687144</v>
       </c>
     </row>
     <row r="40" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E40">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>46163.659884006323</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>67047.51154404429</v>
+      </c>
+      <c r="H40">
         <f t="shared" si="2"/>
-        <v>39</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="0"/>
-        <v>46163.659884006323</v>
-      </c>
-      <c r="G40">
-        <f>SUM(B$2*(1+B$4)^E40)</f>
-        <v>67047.51154404429</v>
-      </c>
-      <c r="H40">
-        <f t="shared" si="1"/>
         <v>201152.97682222116</v>
       </c>
     </row>
     <row r="41" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E41">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>48010.206279366597</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>70399.887121246487</v>
+      </c>
+      <c r="H41">
         <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="0"/>
-        <v>48010.206279366597</v>
-      </c>
-      <c r="G41">
-        <f>SUM(B$2*(1+B$4)^E41)</f>
-        <v>70399.887121246487</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="1"/>
         <v>217245.21496799888</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="133" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="32.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>300</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>300</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="3">
+        <v>40.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="3">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>30</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>300</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>300</v>
+      </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="3">
+        <v>77.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>